<commit_message>
added adding a quotation
</commit_message>
<xml_diff>
--- a/functions/templates/QUOTATION.xlsx
+++ b/functions/templates/QUOTATION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itwab\WebstormProjects\Firebase-Cloud-Functions\functions\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9396E188-DC00-49CA-B450-EA88D0227D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B5A860-221B-4A76-AE19-D1F2355EF3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28560" yWindow="2070" windowWidth="21600" windowHeight="11775" xr2:uid="{865486AF-EF78-404E-A4E3-CFE18021C6DB}"/>
+    <workbookView xWindow="31140" yWindow="2580" windowWidth="21600" windowHeight="11775" xr2:uid="{865486AF-EF78-404E-A4E3-CFE18021C6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -288,17 +288,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -344,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -402,9 +391,6 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -418,13 +404,7 @@
     <xf numFmtId="166" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -443,23 +423,20 @@
     <xf numFmtId="168" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -853,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC825F3-177E-4B74-8210-F411CB8214BE}">
   <dimension ref="B1:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" customHeight="1"/>
@@ -1000,8 +977,11 @@
         <v>8</v>
       </c>
       <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="21" t="e">
+        <f t="shared" ref="F20:F34" si="0">E20*D20</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="25"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1009,9 +989,9 @@
       <c r="L20" s="7"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="27"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="28"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="20"/>
       <c r="F21" s="21"/>
       <c r="G21" s="10"/>
@@ -1019,218 +999,218 @@
     <row r="22" spans="2:12">
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="29"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="27"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="20"/>
-      <c r="D23" s="28"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="20"/>
       <c r="F23" s="21"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="30"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="24"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="32"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="20"/>
-      <c r="D25" s="28"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="33"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="34"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="29"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="26"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="32"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="20"/>
-      <c r="D27" s="28"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="33"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="34"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="24"/>
-      <c r="D28" s="35"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="26"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="2:12">
-      <c r="B29" s="32"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="36"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="33"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="2:12">
-      <c r="B30" s="34"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="24"/>
-      <c r="D30" s="35"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="26"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="32"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="20"/>
-      <c r="D31" s="36"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="33"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="2:12">
-      <c r="B32" s="34"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="24"/>
-      <c r="D32" s="35"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="24"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="26"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="32"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="20"/>
-      <c r="D33" s="37"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="33"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="26"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="43"/>
-      <c r="C35" s="44"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="46" t="e">
+      <c r="F35" s="42" t="e">
         <f>SUM(F19:F34)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C36" s="44"/>
-      <c r="E36" s="45" t="s">
+      <c r="C36" s="40"/>
+      <c r="E36" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="47">
+      <c r="F36" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="14.25" hidden="1" customHeight="1">
-      <c r="C37" s="44"/>
-      <c r="E37" s="45" t="s">
+      <c r="C37" s="40"/>
+      <c r="E37" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F37" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C38" s="44"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="46"/>
+      <c r="C38" s="40"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="42"/>
     </row>
     <row r="39" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C39" s="44"/>
-      <c r="E39" s="45" t="s">
+      <c r="C39" s="40"/>
+      <c r="E39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="46" t="e">
+      <c r="F39" s="42" t="e">
         <f>F35+F36</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C40" s="44"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="50"/>
+      <c r="C40" s="40"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="46"/>
     </row>
     <row r="41" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C41" s="44"/>
-      <c r="F41" s="51"/>
+      <c r="C41" s="40"/>
+      <c r="F41" s="47"/>
     </row>
     <row r="42" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C42" s="44"/>
+      <c r="C42" s="40"/>
     </row>
     <row r="43" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C43" s="44"/>
+      <c r="C43" s="40"/>
     </row>
     <row r="44" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C44" s="44"/>
+      <c r="C44" s="40"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="C45" s="44"/>
+      <c r="C45" s="40"/>
     </row>
     <row r="46" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C46" s="44"/>
+      <c r="C46" s="40"/>
     </row>
     <row r="47" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C47" s="44"/>
+      <c r="C47" s="40"/>
     </row>
     <row r="48" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C48" s="44"/>
+      <c r="C48" s="40"/>
     </row>
     <row r="49" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C49" s="44"/>
+      <c r="C49" s="40"/>
     </row>
     <row r="50" spans="2:7" ht="14.25" customHeight="1">
-      <c r="C50" s="44"/>
+      <c r="C50" s="40"/>
     </row>
     <row r="51" spans="2:7" ht="17.55" customHeight="1">
-      <c r="C51" s="44"/>
+      <c r="C51" s="40"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="C52" s="44"/>
+      <c r="C52" s="40"/>
     </row>
     <row r="53" spans="2:7" ht="20.55" customHeight="1">
-      <c r="C53" s="44"/>
+      <c r="C53" s="40"/>
     </row>
     <row r="54" spans="2:7" ht="14.25" customHeight="1">
-      <c r="B54" s="43"/>
-      <c r="C54" s="44"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="2:7" ht="14.25" customHeight="1">
-      <c r="B55" s="52"/>
-      <c r="C55" s="53"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="3"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="2:7" ht="14.25" customHeight="1">
-      <c r="B56" s="52"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="2"/>
     </row>
     <row r="57" spans="2:7" ht="14.25" customHeight="1">
-      <c r="B57" s="52"/>
+      <c r="B57" s="48"/>
       <c r="C57" s="2"/>
     </row>
     <row r="58" spans="2:7" ht="14.25" customHeight="1">
-      <c r="B58" s="52"/>
+      <c r="B58" s="48"/>
       <c r="C58" s="2"/>
     </row>
     <row r="59" spans="2:7" ht="14.25" customHeight="1">

</xml_diff>